<commit_message>
phase1 update final fix
</commit_message>
<xml_diff>
--- a/faya-api/src/test/resources/Phase1TestData.xlsx
+++ b/faya-api/src/test/resources/Phase1TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/GitHub/faya/fayaapi/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/GitHub/faya/faya-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="28320" windowHeight="16460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="75">
   <si>
     <t>Security Reference Data</t>
   </si>
@@ -43,18 +43,9 @@
     <t>Pricing Data</t>
   </si>
   <si>
-    <t>912828SQ4</t>
-  </si>
-  <si>
     <t>USTN TII .125% 4/15/17</t>
   </si>
   <si>
-    <t>BBFKMW7</t>
-  </si>
-  <si>
-    <t>B85SFQ5</t>
-  </si>
-  <si>
     <t>ITALY GOVT I/L 2.25% 4/17</t>
   </si>
   <si>
@@ -68,33 +59,6 @@
   </si>
   <si>
     <t>DVRN</t>
-  </si>
-  <si>
-    <t>242846AA1</t>
-  </si>
-  <si>
-    <t>735220AR6</t>
-  </si>
-  <si>
-    <t>93978HHQ1</t>
-  </si>
-  <si>
-    <t>246579AF3</t>
-  </si>
-  <si>
-    <t>25154CA20</t>
-  </si>
-  <si>
-    <t>25155DL33</t>
-  </si>
-  <si>
-    <t>64579FYG2</t>
-  </si>
-  <si>
-    <t>646065SM5</t>
-  </si>
-  <si>
-    <t>87638QBX6</t>
   </si>
   <si>
     <t>DECATUR AL IDB NUCOR VR7@</t>
@@ -385,7 +349,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -406,6 +370,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -712,8 +677,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -758,7 +723,7 @@
       </c>
       <c r="E1" s="6"/>
       <c r="M1" s="10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
@@ -776,193 +741,193 @@
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
       <c r="AC1" s="10" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AE2" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="AD3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="20">
+        <v>1111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>49888</v>
@@ -975,11 +940,11 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -991,7 +956,7 @@
         <v>18</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="O4" s="3">
         <v>41974</v>
@@ -1025,22 +990,22 @@
         <v>100</v>
       </c>
       <c r="Y4" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z4" s="18">
         <v>1</v>
       </c>
       <c r="AA4" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB4" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC4" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD4" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE4" s="14">
         <v>2.3000110000000002E-3</v>
@@ -1052,13 +1017,13 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1112</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3">
         <v>44166</v>
@@ -1071,11 +1036,11 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K5">
         <v>100</v>
@@ -1087,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O5" s="3">
         <v>41974</v>
@@ -1121,22 +1086,22 @@
         <v>100</v>
       </c>
       <c r="Y5" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z5" s="18">
         <v>1</v>
       </c>
       <c r="AA5" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB5" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC5" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD5" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE5" s="14">
         <v>2.6000045000000001E-3</v>
@@ -1148,13 +1113,13 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1113</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3">
         <v>56462</v>
@@ -1167,11 +1132,11 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K6">
         <v>100</v>
@@ -1183,7 +1148,7 @@
         <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="O6" s="3">
         <v>41974</v>
@@ -1217,22 +1182,22 @@
         <v>100</v>
       </c>
       <c r="Y6" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z6" s="18">
         <v>1</v>
       </c>
       <c r="AA6" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB6" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC6" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD6" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE6" s="14">
         <v>5.6999860000000006E-3</v>
@@ -1244,13 +1209,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="20">
+        <v>1114</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>48914</v>
@@ -1263,11 +1228,11 @@
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <v>100</v>
@@ -1279,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O7" s="3">
         <v>41974</v>
@@ -1313,22 +1278,22 @@
         <v>100</v>
       </c>
       <c r="Y7" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z7" s="18">
         <v>1</v>
       </c>
       <c r="AA7" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB7" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC7" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD7" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE7" s="14">
         <v>3.0000080000000002E-3</v>
@@ -1340,13 +1305,13 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="20">
+        <v>1115</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3">
         <v>50587</v>
@@ -1359,11 +1324,11 @@
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K8">
         <v>100</v>
@@ -1375,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O8" s="3">
         <v>41974</v>
@@ -1409,22 +1374,22 @@
         <v>100</v>
       </c>
       <c r="Y8" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z8" s="18">
         <v>1</v>
       </c>
       <c r="AA8" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB8" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC8" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD8" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE8" s="14">
         <v>4.2999919999999999E-3</v>
@@ -1436,13 +1401,13 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1116</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
         <v>49857</v>
@@ -1455,11 +1420,11 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K9">
         <v>100</v>
@@ -1471,7 +1436,7 @@
         <v>22</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O9" s="3">
         <v>41974</v>
@@ -1505,22 +1470,22 @@
         <v>100</v>
       </c>
       <c r="Y9" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z9" s="18">
         <v>1</v>
       </c>
       <c r="AA9" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB9" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC9" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD9" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE9" s="14">
         <v>2.4999944999999999E-3</v>
@@ -1532,13 +1497,13 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1117</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="3">
         <v>51105</v>
@@ -1551,11 +1516,11 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K10">
         <v>100</v>
@@ -1567,7 +1532,7 @@
         <v>18</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="O10" s="3">
         <v>41974</v>
@@ -1601,22 +1566,22 @@
         <v>100</v>
       </c>
       <c r="Y10" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z10" s="18">
         <v>1</v>
       </c>
       <c r="AA10" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB10" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC10" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD10" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE10" s="14">
         <v>1.5000040000000001E-3</v>
@@ -1628,13 +1593,13 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1118</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>47437</v>
@@ -1646,10 +1611,10 @@
         <v>0.23999845</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K11">
         <v>100</v>
@@ -1661,7 +1626,7 @@
         <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O11" s="3">
         <v>41974</v>
@@ -1695,22 +1660,22 @@
         <v>100</v>
       </c>
       <c r="Y11" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z11" s="18">
         <v>1</v>
       </c>
       <c r="AA11" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB11" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC11" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD11" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE11" s="14">
         <v>2.3999845000000001E-3</v>
@@ -1724,11 +1689,11 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="20">
+        <v>1119</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D12" s="3">
         <v>42840</v>
@@ -1741,11 +1706,11 @@
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <v>106.0762902</v>
@@ -1757,7 +1722,7 @@
         <v>21</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="O12" s="3">
         <v>41974</v>
@@ -1791,22 +1756,22 @@
         <v>101.22652727810596</v>
       </c>
       <c r="Y12" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z12" s="18">
         <v>1.0479099999999999</v>
       </c>
       <c r="AA12" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB12" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC12" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD12" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE12" s="14">
         <v>-3.8914641607654945E-3</v>
@@ -1820,11 +1785,11 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="20">
+        <v>1119</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D13" s="3">
         <v>42840</v>
@@ -1837,11 +1802,11 @@
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K13">
         <v>106.0762902</v>
@@ -1853,7 +1818,7 @@
         <v>30</v>
       </c>
       <c r="N13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="O13" s="3">
         <v>41974</v>
@@ -1887,22 +1852,22 @@
         <v>101.22652727810596</v>
       </c>
       <c r="Y13" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z13" s="18">
         <v>1.0479099999999999</v>
       </c>
       <c r="AA13" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB13" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC13" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD13" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE13" s="14">
         <v>-3.8914641607654945E-3</v>
@@ -1916,11 +1881,11 @@
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="20">
+        <v>1119</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D14" s="3">
         <v>42840</v>
@@ -1933,11 +1898,11 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K14">
         <v>106.0762902</v>
@@ -1949,7 +1914,7 @@
         <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="O14" s="3">
         <v>41974</v>
@@ -1983,22 +1948,22 @@
         <v>101.22652727810596</v>
       </c>
       <c r="Y14" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z14" s="18">
         <v>1.0479099999999999</v>
       </c>
       <c r="AA14" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB14" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC14" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD14" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE14" s="14">
         <v>-3.8914641607654945E-3</v>
@@ -2010,13 +1975,13 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="20">
+        <v>1120</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D15" s="3">
         <v>49949</v>
@@ -2029,11 +1994,11 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K15">
         <v>100</v>
@@ -2045,7 +2010,7 @@
         <v>18</v>
       </c>
       <c r="N15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="O15" s="3">
         <v>41974</v>
@@ -2079,22 +2044,22 @@
         <v>100</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z15" s="18">
         <v>1</v>
       </c>
       <c r="AA15" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB15" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC15" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD15" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE15" s="14">
         <v>2.0999909999999998E-3</v>
@@ -2106,13 +2071,13 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>1120</v>
+      </c>
+      <c r="C16" t="s">
         <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
       </c>
       <c r="D16">
         <v>49949</v>
@@ -2124,10 +2089,10 @@
         <v>0.20999909999999999</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K16">
         <v>100</v>
@@ -2139,7 +2104,7 @@
         <v>22</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O16" s="3">
         <v>41974</v>
@@ -2173,22 +2138,22 @@
         <v>100</v>
       </c>
       <c r="Y16" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z16" s="18">
         <v>1</v>
       </c>
       <c r="AA16" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB16" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC16" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AD16" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="AE16" s="14">
         <v>2.0999909999999998E-3</v>
@@ -2202,11 +2167,11 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
+      <c r="B17" s="20">
+        <v>1121</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
         <v>45373</v>
@@ -2219,11 +2184,11 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K17">
         <v>116.30485349999999</v>
@@ -2235,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="N17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="O17" s="3">
         <v>41974</v>
@@ -2269,22 +2234,22 @@
         <v>116.30485349999999</v>
       </c>
       <c r="Y17" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z17" s="18">
         <v>1</v>
       </c>
       <c r="AA17" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB17" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC17" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD17" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE17" s="14">
         <v>-1.5005795554410607E-2</v>
@@ -2298,11 +2263,11 @@
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
+      <c r="B18" s="20">
+        <v>1121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3">
         <v>45373</v>
@@ -2315,11 +2280,11 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K18">
         <v>116.30485349999999</v>
@@ -2331,7 +2296,7 @@
         <v>9</v>
       </c>
       <c r="N18" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="O18" s="3">
         <v>41974</v>
@@ -2365,22 +2330,22 @@
         <v>116.30485349999999</v>
       </c>
       <c r="Y18" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z18" s="18">
         <v>1</v>
       </c>
       <c r="AA18" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB18" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC18" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD18" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE18" s="14">
         <v>-1.5005795554410607E-2</v>
@@ -2394,11 +2359,11 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
+      <c r="B19" s="20">
+        <v>1121</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3">
         <v>45373</v>
@@ -2411,11 +2376,11 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K19">
         <v>116.30485349999999</v>
@@ -2427,7 +2392,7 @@
         <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="O19" s="3">
         <v>41974</v>
@@ -2461,22 +2426,22 @@
         <v>116.30485349999999</v>
       </c>
       <c r="Y19" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z19" s="18">
         <v>1</v>
       </c>
       <c r="AA19" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB19" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC19" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD19" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE19" s="14">
         <v>-1.5005795554410607E-2</v>
@@ -2490,11 +2455,11 @@
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
+      <c r="B20" s="20">
+        <v>1121</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3">
         <v>45373</v>
@@ -2507,11 +2472,11 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K20">
         <v>116.30485349999999</v>
@@ -2523,7 +2488,7 @@
         <v>31</v>
       </c>
       <c r="N20" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="O20" s="3">
         <v>41974</v>
@@ -2557,22 +2522,22 @@
         <v>116.30485349999999</v>
       </c>
       <c r="Y20" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z20" s="18">
         <v>1</v>
       </c>
       <c r="AA20" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB20" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC20" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD20" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE20" s="14">
         <v>-1.5005795554410607E-2</v>
@@ -2586,11 +2551,11 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
+      <c r="B21" s="20">
+        <v>1121</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D21" s="3">
         <v>45373</v>
@@ -2603,11 +2568,11 @@
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K21">
         <v>116.30485349999999</v>
@@ -2619,7 +2584,7 @@
         <v>33</v>
       </c>
       <c r="N21" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O21" s="3">
         <v>41974</v>
@@ -2653,22 +2618,22 @@
         <v>116.30485349999999</v>
       </c>
       <c r="Y21" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z21" s="18">
         <v>1</v>
       </c>
       <c r="AA21" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB21" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC21" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD21" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE21" s="14">
         <v>-1.5005795554410607E-2</v>
@@ -2682,11 +2647,11 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
+      <c r="B22" s="20">
+        <v>1122</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" s="3">
         <v>42847</v>
@@ -2699,11 +2664,11 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K22">
         <v>103.3477851</v>
@@ -2715,7 +2680,7 @@
         <v>6</v>
       </c>
       <c r="N22" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="O22" s="3">
         <v>41974</v>
@@ -2749,22 +2714,22 @@
         <v>103.3477851</v>
       </c>
       <c r="Y22" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z22" s="18">
         <v>1</v>
       </c>
       <c r="AA22" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB22" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC22" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD22" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE22" s="14">
         <v>8.33155453769731E-3</v>
@@ -2778,11 +2743,11 @@
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
+      <c r="B23" s="20">
+        <v>1122</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D23" s="3">
         <v>42847</v>
@@ -2795,11 +2760,11 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K23">
         <v>103.3477851</v>
@@ -2811,7 +2776,7 @@
         <v>24</v>
       </c>
       <c r="N23" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="O23" s="3">
         <v>41974</v>
@@ -2845,22 +2810,22 @@
         <v>103.3477851</v>
       </c>
       <c r="Y23" s="18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z23" s="18">
         <v>1</v>
       </c>
       <c r="AA23" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AB23" s="18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC23" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AD23" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AE23" s="14">
         <v>8.33155453769731E-3</v>

</xml_diff>